<commit_message>
fry run on real market on 30 auh for SEP monthly expiry
</commit_message>
<xml_diff>
--- a/strategies/long_straddle/reports/fake_report.xlsx
+++ b/strategies/long_straddle/reports/fake_report.xlsx
@@ -547,7 +547,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -830,81 +830,324 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
         <is>
           <t>NIFTY 50</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>2024-08-29</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="0" t="inlineStr">
         <is>
           <t>13:40:05</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" s="0" t="n">
         <v>25128.7</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="0" t="n">
         <v>64.45</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5" s="0" t="n">
         <v>25.25</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" s="0" t="n">
         <v>89.7</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J5" s="0" t="n">
         <v>2242.5</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K5" s="0" t="n">
         <v>25100</v>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="L5" s="0" t="inlineStr">
         <is>
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="M5" t="n">
+      <c r="M5" s="0" t="n">
         <v>25137.55</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N5" s="0" t="n">
         <v>66.59999999999999</v>
       </c>
-      <c r="O5" t="n">
+      <c r="O5" s="0" t="n">
         <v>25.6</v>
       </c>
-      <c r="P5" t="n">
+      <c r="P5" s="0" t="n">
         <v>92.19999999999999</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="Q5" s="0" t="n">
         <v>2305</v>
       </c>
-      <c r="R5" t="n">
+      <c r="R5" s="0" t="n">
         <v>2.499999999999986</v>
       </c>
-      <c r="S5" t="n">
+      <c r="S5" s="0" t="n">
         <v>62.49999999999955</v>
       </c>
-      <c r="T5" t="n">
+      <c r="T5" s="0" t="n">
         <v>97.088994</v>
       </c>
-      <c r="U5" t="n">
+      <c r="U5" s="0" t="n">
         <v>-34.58899400000045</v>
       </c>
-      <c r="V5" t="n">
+      <c r="V5" s="0" t="n">
         <v>-1.54243005574138</v>
       </c>
-      <c r="W5" t="inlineStr">
+      <c r="W5" s="0" t="inlineStr">
+        <is>
+          <t>TIME_ELAPSED_WHILE_LOOKING_FOR_INITIAL_SL</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>NIFTY BANK</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>09:20:43</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>51401.8</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>876.2</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>630.15</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1506.35</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>22595.25</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>51400</v>
+      </c>
+      <c r="L6" s="0" t="inlineStr">
+        <is>
+          <t>09:20:46</t>
+        </is>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>51394</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>870.2</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>633.4</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>1503.6</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>22554</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>-2.75</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>-41.25</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>91.82704799999999</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>-133.077048</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>-0.5889602814750887</v>
+      </c>
+      <c r="W6" s="0" t="inlineStr">
+        <is>
+          <t>MAX_LOSS_WHILE_LOOKING_FOR_INITIAL_SL</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>NIFTY BANK</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>09:24:08</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>51398.3</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>879.7</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>626.8</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1506.5</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>22597.5</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>51400</v>
+      </c>
+      <c r="L7" s="0" t="inlineStr">
+        <is>
+          <t>09:24:10</t>
+        </is>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>51402.1</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>876.4</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>626.8</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>1503.2</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>22548</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>-3.300000000000182</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>-49.50000000000364</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>91.76662279999996</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>-141.2666228000036</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>-0.6251427051665166</v>
+      </c>
+      <c r="W7" s="0" t="inlineStr">
+        <is>
+          <t>MAX_LOSS_WHILE_LOOKING_FOR_INITIAL_SL</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NIFTY BANK</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>15</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>09:35:01</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>51333.35</v>
+      </c>
+      <c r="G8" t="n">
+        <v>919</v>
+      </c>
+      <c r="H8" t="n">
+        <v>593.45</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1512.45</v>
+      </c>
+      <c r="J8" t="n">
+        <v>22686.75</v>
+      </c>
+      <c r="K8" t="n">
+        <v>51300</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>51392.55</v>
+      </c>
+      <c r="N8" t="n">
+        <v>946.05</v>
+      </c>
+      <c r="O8" t="n">
+        <v>574.95</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1521</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>22815</v>
+      </c>
+      <c r="R8" t="n">
+        <v>8.549999999999955</v>
+      </c>
+      <c r="S8" t="n">
+        <v>128.25</v>
+      </c>
+      <c r="T8" t="n">
+        <v>93.06851119999999</v>
+      </c>
+      <c r="U8" t="n">
+        <v>35.18148880000001</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.1550750495333179</v>
+      </c>
+      <c r="W8" t="inlineStr">
         <is>
           <t>TIME_ELAPSED_WHILE_LOOKING_FOR_INITIAL_SL</t>
         </is>

</xml_diff>